<commit_message>
MCU Change: SAMC21 -> SAM4S
</commit_message>
<xml_diff>
--- a/Datasheets/ATSAM4S/Pinout.xlsx
+++ b/Datasheets/ATSAM4S/Pinout.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\eWheel\Datasheets\ATSAM4S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EA9D593-1B5F-4D37-9DE7-FDFAD3A2242A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3458D6-9832-4B97-A8AB-DF66F9C43007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{9FC1F0F0-5339-4F91-A99A-A80FF950A0A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{9FC1F0F0-5339-4F91-A99A-A80FF950A0A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
   <si>
     <t>PA17</t>
   </si>
@@ -102,9 +102,6 @@
     <t>PA28</t>
   </si>
   <si>
-    <t>PIN</t>
-  </si>
-  <si>
     <t>PA01</t>
   </si>
   <si>
@@ -154,13 +151,259 @@
   </si>
   <si>
     <t>PB07</t>
+  </si>
+  <si>
+    <t>PB04</t>
+  </si>
+  <si>
+    <t>Peripheral A</t>
+  </si>
+  <si>
+    <t>Peripheral B</t>
+  </si>
+  <si>
+    <t>Peripheral C</t>
+  </si>
+  <si>
+    <t>NPCS1</t>
+  </si>
+  <si>
+    <t>PCK2</t>
+  </si>
+  <si>
+    <t>MCDA1</t>
+  </si>
+  <si>
+    <t>PWMH1</t>
+  </si>
+  <si>
+    <t>TIOB0</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>TWD0</t>
+  </si>
+  <si>
+    <t>NPCS3</t>
+  </si>
+  <si>
+    <t>RI1</t>
+  </si>
+  <si>
+    <t>TCLK2</t>
+  </si>
+  <si>
+    <t>MCCK</t>
+  </si>
+  <si>
+    <t>DTR1</t>
+  </si>
+  <si>
+    <t>TIOB2</t>
+  </si>
+  <si>
+    <t>MCDA3</t>
+  </si>
+  <si>
+    <t>RXD0</t>
+  </si>
+  <si>
+    <t>CTS0</t>
+  </si>
+  <si>
+    <t>ADTRG</t>
+  </si>
+  <si>
+    <t>UTXD0</t>
+  </si>
+  <si>
+    <t>NPCS2</t>
+  </si>
+  <si>
+    <t>PWMFI1</t>
+  </si>
+  <si>
+    <t>PWMH0</t>
+  </si>
+  <si>
+    <t>TIOA0</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>PWMH2</t>
+  </si>
+  <si>
+    <t>SCK0</t>
+  </si>
+  <si>
+    <t>DATRG</t>
+  </si>
+  <si>
+    <t>PWML2</t>
+  </si>
+  <si>
+    <t>MCDA0</t>
+  </si>
+  <si>
+    <t>DSR1</t>
+  </si>
+  <si>
+    <t>TCLK1</t>
+  </si>
+  <si>
+    <t>MCCDA</t>
+  </si>
+  <si>
+    <t>TWCK0</t>
+  </si>
+  <si>
+    <t>TCLK0</t>
+  </si>
+  <si>
+    <t>TXD0</t>
+  </si>
+  <si>
+    <t>PCK0</t>
+  </si>
+  <si>
+    <t>RTS0</t>
+  </si>
+  <si>
+    <t>PWMH3</t>
+  </si>
+  <si>
+    <t>URXD0</t>
+  </si>
+  <si>
+    <t>PWMFI0</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>PCK1</t>
+  </si>
+  <si>
+    <t>RXD1</t>
+  </si>
+  <si>
+    <t>TXD1</t>
+  </si>
+  <si>
+    <t>NCS2</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>PWML1</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>TIOA1</t>
+  </si>
+  <si>
+    <t>PWML3</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>CTS1</t>
+  </si>
+  <si>
+    <t>A23</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>RK</t>
+  </si>
+  <si>
+    <t>PWML0</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>SCK1</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>TIOB1</t>
+  </si>
+  <si>
+    <t>SPCK</t>
+  </si>
+  <si>
+    <t>RTS1</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>DCD1</t>
+  </si>
+  <si>
+    <t>TIOA2</t>
+  </si>
+  <si>
+    <t>MCDA2</t>
+  </si>
+  <si>
+    <t>NPCS0</t>
+  </si>
+  <si>
+    <t>TWCK1</t>
+  </si>
+  <si>
+    <t>TWD1</t>
+  </si>
+  <si>
+    <t>URXD1</t>
+  </si>
+  <si>
+    <t>UTXD1</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>PIO</t>
+  </si>
+  <si>
+    <t>TWI</t>
+  </si>
+  <si>
+    <t>UART</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,19 +417,94 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -195,8 +513,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -511,221 +846,586 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA07D8AB-B5BF-43B3-B4F5-F93C011F1C11}">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A4:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G23:G24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="3"/>
+      <c r="S6" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="N8" s="4"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O9" s="8"/>
+      <c r="P9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="O10" s="8"/>
+      <c r="P10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="L11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O11" s="8"/>
+      <c r="P11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R11" s="3"/>
+      <c r="S11" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="U11" s="4"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="L12" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="L13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="O13" s="8"/>
+      <c r="P13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
+      <c r="R14" s="3"/>
+      <c r="S14" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U14" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1" xr:uid="{28B0FD35-A84C-4D7F-A9DB-DA5C0AB76137}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A40">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated PinAssignment on SAM4S-Board
</commit_message>
<xml_diff>
--- a/Datasheets/ATSAM4S/Pinout.xlsx
+++ b/Datasheets/ATSAM4S/Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\eWheel\Datasheets\ATSAM4S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3458D6-9832-4B97-A8AB-DF66F9C43007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB848E0-93D2-4182-B570-DE41DFB2097F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{9FC1F0F0-5339-4F91-A99A-A80FF950A0A4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="124">
   <si>
     <t>PA17</t>
   </si>
@@ -397,6 +397,15 @@
   </si>
   <si>
     <t>UART</t>
+  </si>
+  <si>
+    <t>USART</t>
+  </si>
+  <si>
+    <t>VESC.USART</t>
+  </si>
+  <si>
+    <t>W25Q128.SPI</t>
   </si>
 </sst>
 </file>
@@ -433,7 +442,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +485,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -513,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -532,6 +547,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -849,7 +868,7 @@
   <dimension ref="A4:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:F16"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,13 +1107,16 @@
       <c r="H8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="13" t="s">
         <v>67</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="K8" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="L8" s="13" t="s">
         <v>84</v>
       </c>
       <c r="M8" s="3" t="s">
@@ -1146,7 +1168,7 @@
       <c r="J9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="13" t="s">
         <v>85</v>
       </c>
       <c r="M9" s="5" t="s">
@@ -1163,7 +1185,7 @@
         <v>10</v>
       </c>
       <c r="R9" s="3"/>
-      <c r="S9" s="3" t="s">
+      <c r="S9" s="13" t="s">
         <v>102</v>
       </c>
       <c r="T9" s="3" t="s">
@@ -1174,7 +1196,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1191,7 +1213,7 @@
         <v>21</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="13" t="s">
         <v>71</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -1228,14 +1250,16 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="12" t="s">
+        <v>122</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1266,7 +1290,9 @@
       <c r="Q11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R11" s="3"/>
+      <c r="R11" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="S11" s="5" t="s">
         <v>106</v>
       </c>
@@ -1290,8 +1316,10 @@
       <c r="F12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>76</v>
       </c>
       <c r="I12" s="3" t="s">
@@ -1305,7 +1333,9 @@
         <v>66</v>
       </c>
       <c r="N12" s="4"/>
-      <c r="O12" s="8"/>
+      <c r="O12" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="P12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1313,7 +1343,7 @@
         <v>13</v>
       </c>
       <c r="R12" s="3"/>
-      <c r="S12" s="3" t="s">
+      <c r="S12" s="13" t="s">
         <v>107</v>
       </c>
       <c r="T12" s="3" t="s">
@@ -1324,7 +1354,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="13" t="s">
         <v>58</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1339,14 +1369,14 @@
         <v>29</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="13" t="s">
         <v>78</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>79</v>
       </c>
       <c r="J13" s="4"/>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="13" t="s">
         <v>94</v>
       </c>
       <c r="M13" s="3" t="s">
@@ -1363,7 +1393,7 @@
         <v>14</v>
       </c>
       <c r="R13" s="3"/>
-      <c r="S13" s="3" t="s">
+      <c r="S13" s="13" t="s">
         <v>109</v>
       </c>
       <c r="T13" s="3" t="s">
@@ -1407,14 +1437,18 @@
         <v>46</v>
       </c>
       <c r="N14" s="4"/>
-      <c r="O14" s="8"/>
+      <c r="O14" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="P14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R14" s="3"/>
+      <c r="R14" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="S14" s="5" t="s">
         <v>112</v>
       </c>

</xml_diff>

<commit_message>
Added Datasheet for opto-isolation and BNO055
</commit_message>
<xml_diff>
--- a/Datasheets/ATSAM4S/Pinout.xlsx
+++ b/Datasheets/ATSAM4S/Pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\eWheel\Datasheets\ATSAM4S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB848E0-93D2-4182-B570-DE41DFB2097F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D67E6BC-6D9C-4497-9C57-B4780F10E169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{9FC1F0F0-5339-4F91-A99A-A80FF950A0A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{9FC1F0F0-5339-4F91-A99A-A80FF950A0A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="125">
   <si>
     <t>PA17</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>W25Q128.SPI</t>
+  </si>
+  <si>
+    <t>BNO055.UART</t>
   </si>
 </sst>
 </file>
@@ -868,7 +871,7 @@
   <dimension ref="A4:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="N17" sqref="M17:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1126,9 @@
         <v>83</v>
       </c>
       <c r="N8" s="4"/>
-      <c r="O8" s="8"/>
+      <c r="O8" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="P8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1177,7 +1182,9 @@
       <c r="N9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="O9" s="8"/>
+      <c r="O9" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="P9" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Implemented DriveController & UART for CP2102
DriveController:
- 100hz update of IMU data
UART for CP2102
- Configuration of peripheral for 921600 baud communication
</commit_message>
<xml_diff>
--- a/Datasheets/ATSAM4S/Pinout.xlsx
+++ b/Datasheets/ATSAM4S/Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\eWheel\Datasheets\ATSAM4S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D67E6BC-6D9C-4497-9C57-B4780F10E169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB203E1C-22AA-4FF7-9ECE-4FD401B01688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{9FC1F0F0-5339-4F91-A99A-A80FF950A0A4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="126">
   <si>
     <t>PA17</t>
   </si>
@@ -405,17 +405,21 @@
     <t>VESC.USART</t>
   </si>
   <si>
-    <t>W25Q128.SPI</t>
-  </si>
-  <si>
     <t>BNO055.UART</t>
+  </si>
+  <si>
+    <t>W25Q128.SPI
+ADS1118.SPI</t>
+  </si>
+  <si>
+    <t>CP2102.UART</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,6 +443,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -531,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -554,6 +565,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -871,7 +885,7 @@
   <dimension ref="A4:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="M17:N17"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,14 +1032,18 @@
         <v>61</v>
       </c>
       <c r="N6" s="4"/>
-      <c r="O6" s="8"/>
+      <c r="O6" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="P6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="3"/>
+      <c r="R6" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="S6" s="7" t="s">
         <v>116</v>
       </c>
@@ -1127,7 +1145,7 @@
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>1</v>
@@ -1183,7 +1201,7 @@
         <v>86</v>
       </c>
       <c r="O9" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>2</v>
@@ -1256,7 +1274,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -1297,8 +1315,8 @@
       <c r="Q11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R11" s="5" t="s">
-        <v>123</v>
+      <c r="R11" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="S11" s="5" t="s">
         <v>106</v>
@@ -1308,7 +1326,7 @@
       </c>
       <c r="U11" s="4"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>114</v>
       </c>
@@ -1340,8 +1358,8 @@
         <v>66</v>
       </c>
       <c r="N12" s="4"/>
-      <c r="O12" s="5" t="s">
-        <v>123</v>
+      <c r="O12" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>5</v>
@@ -1410,7 +1428,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>60</v>
       </c>
@@ -1444,8 +1462,8 @@
         <v>46</v>
       </c>
       <c r="N14" s="4"/>
-      <c r="O14" s="5" t="s">
-        <v>123</v>
+      <c r="O14" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>7</v>
@@ -1453,8 +1471,8 @@
       <c r="Q14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R14" s="5" t="s">
-        <v>123</v>
+      <c r="R14" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="S14" s="5" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
Added Datasheet for Distancesensor
</commit_message>
<xml_diff>
--- a/Datasheets/ATSAM4S/Pinout.xlsx
+++ b/Datasheets/ATSAM4S/Pinout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\eWheel\Datasheets\ATSAM4S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F86BF6-B685-49FF-80C3-E7531FFA627F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668A2D3A-C3DF-4E3B-A141-359F792D2F51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{9FC1F0F0-5339-4F91-A99A-A80FF950A0A4}"/>
   </bookViews>
@@ -891,7 +891,7 @@
   <dimension ref="A4:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +976,9 @@
       <c r="C5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1451,9 +1453,7 @@
       <c r="F14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>127</v>
-      </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="7" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
Implemented UART for CC41A
</commit_message>
<xml_diff>
--- a/Datasheets/ATSAM4S/Pinout.xlsx
+++ b/Datasheets/ATSAM4S/Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\eWheel\Datasheets\ATSAM4S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668A2D3A-C3DF-4E3B-A141-359F792D2F51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE04227E-90C0-4689-AA03-ADE83916855C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{9FC1F0F0-5339-4F91-A99A-A80FF950A0A4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="129">
   <si>
     <t>PA17</t>
   </si>
@@ -419,6 +419,9 @@
   </si>
   <si>
     <t>ADS1118.SPI</t>
+  </si>
+  <si>
+    <t>CC41A.UART</t>
   </si>
 </sst>
 </file>
@@ -891,7 +894,7 @@
   <dimension ref="A4:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,14 +1449,18 @@
       <c r="C14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="H14" s="7" t="s">
         <v>80</v>
       </c>

</xml_diff>